<commit_message>
Update to latest input spreadsheet
Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220415 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220415 ITR Tool Sample Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AE4771-8E0E-844B-99C5-862C5AF799F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97047AF6-7681-C646-8DE3-DD48CF743736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30160" yWindow="24140" windowWidth="50660" windowHeight="23200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -583,7 +583,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="324">
   <si>
     <t>Data field</t>
   </si>
@@ -1678,9 +1678,6 @@
   </si>
   <si>
     <t>Asia</t>
-  </si>
-  <si>
-    <t>megaJPY</t>
   </si>
   <si>
     <t>JP</t>
@@ -2019,7 +2016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2190,6 +2187,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="8" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3454,10 +3452,10 @@
   <dimension ref="A1:AZ61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M50" sqref="M50"/>
+      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -7230,7 +7228,7 @@
         <v>321</v>
       </c>
       <c r="D31" s="60" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>322</v>
@@ -7242,27 +7240,30 @@
         <v>64</v>
       </c>
       <c r="H31" s="60" t="s">
-        <v>323</v>
+        <v>65</v>
       </c>
       <c r="I31" s="60">
         <v>2019</v>
       </c>
       <c r="J31" s="60">
-        <v>879400</v>
+        <f>879400*1000000/107.92</f>
+        <v>8148628613.7879906</v>
       </c>
       <c r="K31" s="60">
-        <v>5921500</v>
+        <f>5921500*1000000/107.92</f>
+        <v>54869347664.936989</v>
       </c>
       <c r="L31" s="60">
-        <f>M31+289549</f>
-        <v>3657690</v>
+        <f>M31+289549*1000000/107.92</f>
+        <v>33892605633.802818</v>
       </c>
       <c r="M31" s="60">
-        <f>J31+2488741</f>
-        <v>3368141</v>
+        <f>J31+2488741*1000000/107.92</f>
+        <v>31209608969.607117</v>
       </c>
       <c r="N31" s="60">
-        <v>7444965</v>
+        <f>7444965*1000000/107.92</f>
+        <v>68985961823.573013</v>
       </c>
       <c r="O31" s="60" t="s">
         <v>141</v>
@@ -7978,7 +7979,7 @@
         <v>240</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>293</v>
+        <v>322</v>
       </c>
       <c r="F37" s="60" t="s">
         <v>166</v>
@@ -8965,6 +8966,9 @@
       <c r="I45" s="60">
         <v>2019</v>
       </c>
+      <c r="J45" s="90">
+        <v>50030000000</v>
+      </c>
       <c r="K45" s="60">
         <v>10175225448.55982</v>
       </c>
@@ -9085,6 +9089,9 @@
       <c r="I46" s="60">
         <v>2019</v>
       </c>
+      <c r="J46" s="20">
+        <v>590000000</v>
+      </c>
       <c r="K46" s="60">
         <v>7294055000</v>
       </c>
@@ -9206,6 +9213,9 @@
       </c>
       <c r="I47" s="60">
         <v>2019</v>
+      </c>
+      <c r="J47" s="20">
+        <v>352130000</v>
       </c>
       <c r="K47" s="60">
         <v>10192818000</v>
@@ -10323,7 +10333,7 @@
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
@@ -14031,7 +14041,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>161895</v>
+        <v>193380</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -14049,7 +14059,7 @@
       </c>
       <c r="E3" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>93546</v>
+        <v>39627</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -14067,7 +14077,7 @@
       </c>
       <c r="E4" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>127523</v>
+        <v>222167</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -14085,7 +14095,7 @@
       </c>
       <c r="E5" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>117151</v>
+        <v>74380</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -14103,7 +14113,7 @@
       </c>
       <c r="E6" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>166478</v>
+        <v>192540</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -14121,7 +14131,7 @@
       </c>
       <c r="E7" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>52761</v>
+        <v>202760</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -14139,7 +14149,7 @@
       </c>
       <c r="E8" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>65938</v>
+        <v>215718</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -14157,7 +14167,7 @@
       </c>
       <c r="E9" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>117016</v>
+        <v>95944</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -14175,7 +14185,7 @@
       </c>
       <c r="E10" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>79318</v>
+        <v>162679</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -14193,7 +14203,7 @@
       </c>
       <c r="E11" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>247382</v>
+        <v>144518</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -14211,7 +14221,7 @@
       </c>
       <c r="E12" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>148416</v>
+        <v>243583</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -14229,7 +14239,7 @@
       </c>
       <c r="E13" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>62323</v>
+        <v>113845</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -14247,7 +14257,7 @@
       </c>
       <c r="E14" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>188688</v>
+        <v>233116</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -14265,7 +14275,7 @@
       </c>
       <c r="E15" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>52146</v>
+        <v>69204</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -14283,7 +14293,7 @@
       </c>
       <c r="E16" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>169954</v>
+        <v>226606</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -14301,7 +14311,7 @@
       </c>
       <c r="E17" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>162565</v>
+        <v>137627</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -14319,7 +14329,7 @@
       </c>
       <c r="E18" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>78849</v>
+        <v>175633</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -14337,7 +14347,7 @@
       </c>
       <c r="E19" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>214062</v>
+        <v>57344</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -14355,7 +14365,7 @@
       </c>
       <c r="E20" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>42401</v>
+        <v>166972</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -14373,7 +14383,7 @@
       </c>
       <c r="E21" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>200225</v>
+        <v>162715</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -14391,7 +14401,7 @@
       </c>
       <c r="E22" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>99244</v>
+        <v>176355</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -14409,7 +14419,7 @@
       </c>
       <c r="E23" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>74279</v>
+        <v>144635</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -14427,7 +14437,7 @@
       </c>
       <c r="E24" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>73526</v>
+        <v>240792</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -14445,7 +14455,7 @@
       </c>
       <c r="E25" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>56728</v>
+        <v>229459</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -14463,7 +14473,7 @@
       </c>
       <c r="E26" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>41518</v>
+        <v>62891</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -14481,7 +14491,7 @@
       </c>
       <c r="E27" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>226979</v>
+        <v>156105</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -14499,7 +14509,7 @@
       </c>
       <c r="E28" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>128358</v>
+        <v>169686</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -14517,7 +14527,7 @@
       </c>
       <c r="E29" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>35374</v>
+        <v>222303</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -14535,7 +14545,7 @@
       </c>
       <c r="E30" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>135018</v>
+        <v>111348</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -14553,7 +14563,7 @@
       </c>
       <c r="E31" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>235166</v>
+        <v>83107</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -14571,7 +14581,7 @@
       </c>
       <c r="E32" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>134735</v>
+        <v>96479</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -14589,7 +14599,7 @@
       </c>
       <c r="E33" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>223755</v>
+        <v>122002</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -14607,7 +14617,7 @@
       </c>
       <c r="E34" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>129205</v>
+        <v>220331</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -14625,7 +14635,7 @@
       </c>
       <c r="E35" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>77652</v>
+        <v>195651</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -14643,7 +14653,7 @@
       </c>
       <c r="E36" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>65246</v>
+        <v>199157</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -14661,7 +14671,7 @@
       </c>
       <c r="E37" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>187832</v>
+        <v>74163</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -14679,7 +14689,7 @@
       </c>
       <c r="E38" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>55659</v>
+        <v>74057</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -14697,7 +14707,7 @@
       </c>
       <c r="E39" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>143811</v>
+        <v>213720</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -14715,7 +14725,7 @@
       </c>
       <c r="E40" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>248941</v>
+        <v>184693</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -14733,7 +14743,7 @@
       </c>
       <c r="E41" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>76971</v>
+        <v>117539</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -14751,7 +14761,7 @@
       </c>
       <c r="E42" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>149707</v>
+        <v>175770</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -14769,7 +14779,7 @@
       </c>
       <c r="E43" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>249215</v>
+        <v>134503</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="60" customFormat="1">
@@ -14787,7 +14797,7 @@
       </c>
       <c r="E44" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>57115</v>
+        <v>146774</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -14805,7 +14815,7 @@
       </c>
       <c r="E45" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>103454</v>
+        <v>225608</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -14823,7 +14833,7 @@
       </c>
       <c r="E46" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>86470</v>
+        <v>98371</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -14841,7 +14851,7 @@
       </c>
       <c r="E47" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>197146</v>
+        <v>75331</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -14859,7 +14869,7 @@
       </c>
       <c r="E48" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>186791</v>
+        <v>204958</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -14877,7 +14887,7 @@
       </c>
       <c r="E49" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>242679</v>
+        <v>232597</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -14895,7 +14905,7 @@
       </c>
       <c r="E50" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>111916</v>
+        <v>170409</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -14913,7 +14923,7 @@
       </c>
       <c r="E51" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>53489</v>
+        <v>177250</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -14931,7 +14941,7 @@
       </c>
       <c r="E52" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>45957</v>
+        <v>215961</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -14949,7 +14959,7 @@
       </c>
       <c r="E53" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>236587</v>
+        <v>174962</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -14967,7 +14977,7 @@
       </c>
       <c r="E54" s="60">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>46170</v>
+        <v>241387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove Exelon Corp from target data - target already expired
Signed-off-by: David Kroon <35101727+dp90@users.noreply.github.com>
Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220415 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220415 ITR Tool Sample Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\FC\DSI\Team\Sasha\sasha_code\ITR_develop\examples\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ITR\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462DCCBD-3ECF-4AF1-91A5-26172CA4782C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAC7F64-845E-44B9-863E-EB31A7241B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -176,9 +176,9 @@
     </comment>
     <comment ref="A50" authorId="1" shapeId="0" xr:uid="{1552FDB1-B469-5E43-9D59-0C000C5BD6F5}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Created target based on ME Netzero goal</t>
       </text>
     </comment>
@@ -328,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{E1E20C21-AC41-454F-BD00-E2E3A76147CB}">
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{E1E20C21-AC41-454F-BD00-E2E3A76147CB}">
       <text>
         <r>
           <rPr>
@@ -361,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{D7FC3687-67D6-B94A-81A4-A3F0B5E62612}">
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{D7FC3687-67D6-B94A-81A4-A3F0B5E62612}">
       <text>
         <r>
           <rPr>
@@ -395,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{D6EF40F2-AAE1-0D4C-AB96-6234B272A95B}">
+    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{D6EF40F2-AAE1-0D4C-AB96-6234B272A95B}">
       <text>
         <r>
           <rPr>
@@ -429,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{3621CB18-1100-1A47-8F98-EC355E02058C}">
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{3621CB18-1100-1A47-8F98-EC355E02058C}">
       <text>
         <r>
           <rPr>
@@ -463,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F52" authorId="0" shapeId="0" xr:uid="{B523BD91-66ED-C74B-BC50-E9F5516DC079}">
+    <comment ref="F51" authorId="0" shapeId="0" xr:uid="{B523BD91-66ED-C74B-BC50-E9F5516DC079}">
       <text>
         <r>
           <rPr>
@@ -496,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F57" authorId="0" shapeId="0" xr:uid="{89150159-53A4-8045-B72C-0B04D7E51127}">
+    <comment ref="F56" authorId="0" shapeId="0" xr:uid="{89150159-53A4-8045-B72C-0B04D7E51127}">
       <text>
         <r>
           <rPr>
@@ -529,7 +529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A61" authorId="0" shapeId="0" xr:uid="{A877392E-78F0-6846-8FB8-D6E550780DF8}">
+    <comment ref="A60" authorId="0" shapeId="0" xr:uid="{A877392E-78F0-6846-8FB8-D6E550780DF8}">
       <text>
         <r>
           <rPr>
@@ -562,19 +562,19 @@
         </r>
       </text>
     </comment>
-    <comment ref="D65" authorId="1" shapeId="0" xr:uid="{8747483F-B5A8-A24A-A61D-346EDF701B94}">
+    <comment ref="D64" authorId="1" shapeId="0" xr:uid="{8747483F-B5A8-A24A-A61D-346EDF701B94}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Announced March 2022</t>
       </text>
     </comment>
-    <comment ref="L65" authorId="2" shapeId="0" xr:uid="{4D3E799C-4A4B-294D-9638-E65AF3840917}">
+    <comment ref="L64" authorId="2" shapeId="0" xr:uid="{4D3E799C-4A4B-294D-9638-E65AF3840917}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Just a guess</t>
       </text>
     </comment>
@@ -583,7 +583,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="323">
   <si>
     <t>Data field</t>
   </si>
@@ -1576,9 +1576,6 @@
   </si>
   <si>
     <t>TWh</t>
-  </si>
-  <si>
-    <t>kt CO2</t>
   </si>
   <si>
     <t>company_isin</t>
@@ -2190,7 +2187,7 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3104,7 +3101,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3408,10 +3405,10 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D65" dT="2022-04-17T20:41:53.75" personId="{5980BEB0-FDC7-2249-B312-9B671A9E62E0}" id="{8747483F-B5A8-A24A-A61D-346EDF701B94}">
+  <threadedComment ref="D64" dT="2022-04-17T20:41:53.75" personId="{5980BEB0-FDC7-2249-B312-9B671A9E62E0}" id="{8747483F-B5A8-A24A-A61D-346EDF701B94}">
     <text>Announced March 2022</text>
   </threadedComment>
-  <threadedComment ref="L65" dT="2022-04-17T20:41:35.41" personId="{5980BEB0-FDC7-2249-B312-9B671A9E62E0}" id="{4D3E799C-4A4B-294D-9638-E65AF3840917}">
+  <threadedComment ref="L64" dT="2022-04-17T20:41:35.41" personId="{5980BEB0-FDC7-2249-B312-9B671A9E62E0}" id="{4D3E799C-4A4B-294D-9638-E65AF3840917}">
     <text>Just a guess</text>
   </threadedComment>
 </ThreadedComments>
@@ -3423,7 +3420,7 @@
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="20" spans="12:18">
       <c r="L20" s="2"/>
@@ -3451,31 +3448,31 @@
   </sheetPr>
   <dimension ref="A1:AZ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F54" sqref="F54"/>
+      <selection pane="bottomRight" activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="24"/>
-    <col min="7" max="7" width="16.44140625" style="4"/>
-    <col min="9" max="9" width="16.44140625" style="5"/>
-    <col min="14" max="14" width="25.77734375" customWidth="1"/>
-    <col min="15" max="15" width="25.77734375" style="60" customWidth="1"/>
-    <col min="16" max="16" width="22.109375" customWidth="1"/>
-    <col min="17" max="21" width="16.44140625" customWidth="1"/>
-    <col min="22" max="22" width="16.44140625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="16.44140625" style="36" customWidth="1"/>
-    <col min="24" max="29" width="16.44140625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="16.44140625" style="36" customWidth="1"/>
-    <col min="31" max="37" width="16.44140625" style="2" customWidth="1"/>
-    <col min="38" max="44" width="16.44140625" style="2"/>
-    <col min="45" max="49" width="16.77734375" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="16.44140625" style="2"/>
+    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="24"/>
+    <col min="7" max="7" width="16.42578125" style="4"/>
+    <col min="9" max="9" width="16.42578125" style="5"/>
+    <col min="14" max="14" width="25.7109375" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" style="60" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" customWidth="1"/>
+    <col min="17" max="21" width="16.42578125" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" style="36" customWidth="1"/>
+    <col min="24" max="29" width="16.42578125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="36" customWidth="1"/>
+    <col min="31" max="37" width="16.42578125" style="2" customWidth="1"/>
+    <col min="38" max="44" width="16.42578125" style="2"/>
+    <col min="45" max="49" width="16.7109375" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="16.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" s="3" customFormat="1">
@@ -4624,13 +4621,13 @@
     </row>
     <row r="10" spans="1:52" s="60" customFormat="1">
       <c r="A10" s="60" t="s">
+        <v>296</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="60" t="s">
         <v>298</v>
-      </c>
-      <c r="C10" s="60" t="s">
-        <v>299</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>61</v>
@@ -5594,13 +5591,13 @@
     </row>
     <row r="18" spans="1:49">
       <c r="A18" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>61</v>
@@ -6477,7 +6474,7 @@
         <v>210</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F25" s="60" t="s">
         <v>166</v>
@@ -7096,13 +7093,13 @@
     </row>
     <row r="30" spans="1:49" s="60" customFormat="1">
       <c r="A30" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="60" t="s">
         <v>304</v>
-      </c>
-      <c r="C30" s="60" t="s">
-        <v>305</v>
       </c>
       <c r="D30" s="60" t="s">
         <v>61</v>
@@ -7219,19 +7216,19 @@
     </row>
     <row r="31" spans="1:49" s="60" customFormat="1">
       <c r="A31" s="60" t="s">
+        <v>318</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="60" t="s">
         <v>320</v>
       </c>
-      <c r="C31" s="60" t="s">
+      <c r="D31" s="60" t="s">
+        <v>322</v>
+      </c>
+      <c r="E31" s="26" t="s">
         <v>321</v>
-      </c>
-      <c r="D31" s="60" t="s">
-        <v>323</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>322</v>
       </c>
       <c r="F31" s="60" t="s">
         <v>166</v>
@@ -7349,13 +7346,13 @@
     </row>
     <row r="32" spans="1:49" s="60" customFormat="1">
       <c r="A32" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="60" t="s">
         <v>307</v>
-      </c>
-      <c r="C32" s="60" t="s">
-        <v>308</v>
       </c>
       <c r="D32" s="60" t="s">
         <v>61</v>
@@ -7979,7 +7976,7 @@
         <v>240</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F37" s="60" t="s">
         <v>166</v>
@@ -9188,13 +9185,13 @@
     </row>
     <row r="47" spans="1:49" s="60" customFormat="1">
       <c r="A47" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="C47" s="60" t="s">
         <v>295</v>
-      </c>
-      <c r="C47" s="60" t="s">
-        <v>296</v>
       </c>
       <c r="D47" s="60" t="s">
         <v>268</v>
@@ -9548,13 +9545,13 @@
     </row>
     <row r="50" spans="1:49" s="60" customFormat="1">
       <c r="A50" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="60" t="s">
         <v>311</v>
-      </c>
-      <c r="C50" s="60" t="s">
-        <v>312</v>
       </c>
       <c r="D50" s="60" t="s">
         <v>147</v>
@@ -9668,13 +9665,13 @@
     </row>
     <row r="51" spans="1:49" s="60" customFormat="1">
       <c r="A51" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="60" t="s">
         <v>314</v>
-      </c>
-      <c r="C51" s="60" t="s">
-        <v>315</v>
       </c>
       <c r="D51" s="60" t="s">
         <v>61</v>
@@ -9914,13 +9911,13 @@
     </row>
     <row r="53" spans="1:49" s="60" customFormat="1">
       <c r="A53" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="60" t="s">
         <v>317</v>
-      </c>
-      <c r="C53" s="60" t="s">
-        <v>318</v>
       </c>
       <c r="D53" s="60" t="s">
         <v>61</v>
@@ -10330,28 +10327,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="60" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="60"/>
-    <col min="4" max="4" width="16.44140625" style="26"/>
-    <col min="5" max="5" width="17.44140625" style="26" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" style="60" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="60"/>
+    <col min="4" max="4" width="16.42578125" style="26"/>
+    <col min="5" max="5" width="17.42578125" style="26" customWidth="1"/>
     <col min="6" max="7" width="24" style="60" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" style="20" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" style="60" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="60" customWidth="1"/>
     <col min="10" max="10" width="24" style="60" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" style="60" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" style="60" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="60" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -10365,7 +10362,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>122</v>
@@ -10818,13 +10815,13 @@
     </row>
     <row r="14" spans="1:12" s="60" customFormat="1">
       <c r="A14" s="60" t="s">
+        <v>296</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="60" t="s">
         <v>298</v>
-      </c>
-      <c r="C14" s="60" t="s">
-        <v>299</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26" t="s">
@@ -11144,13 +11141,13 @@
     </row>
     <row r="23" spans="1:12" s="60" customFormat="1">
       <c r="A23" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B23" s="60" t="s">
         <v>300</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="C23" s="60" t="s">
         <v>301</v>
-      </c>
-      <c r="C23" s="60" t="s">
-        <v>302</v>
       </c>
       <c r="D23" s="26">
         <v>2045</v>
@@ -11332,45 +11329,48 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="60" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C28" s="60" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E28" s="26" t="s">
         <v>282</v>
       </c>
       <c r="F28" s="60" t="s">
-        <v>283</v>
+        <v>281</v>
+      </c>
+      <c r="G28" s="60">
+        <v>2015</v>
       </c>
       <c r="H28" s="20">
-        <v>2015</v>
+        <v>2005</v>
       </c>
       <c r="I28" s="60">
-        <v>1050</v>
+        <v>86403130</v>
       </c>
       <c r="J28" s="70" t="s">
-        <v>289</v>
+        <v>141</v>
       </c>
       <c r="K28" s="60">
-        <v>2022</v>
+        <v>2045</v>
       </c>
       <c r="L28" s="74">
-        <v>0.15</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="60" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C29" s="60" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E29" s="26" t="s">
         <v>282</v>
@@ -11379,121 +11379,119 @@
         <v>281</v>
       </c>
       <c r="G29" s="60">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="H29" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I29" s="60">
-        <v>86403130</v>
+        <v>2019</v>
+      </c>
+      <c r="I29" s="77">
+        <v>11925000</v>
       </c>
       <c r="J29" s="70" t="s">
         <v>141</v>
       </c>
       <c r="K29" s="60">
-        <v>2045</v>
+        <v>2035</v>
       </c>
       <c r="L29" s="74">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="60" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C30" s="60" t="s">
-        <v>206</v>
+        <v>209</v>
+      </c>
+      <c r="D30" s="26">
+        <v>2050</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>282</v>
+        <v>66</v>
       </c>
       <c r="F30" s="60" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G30" s="60">
+        <v>2022</v>
+      </c>
+      <c r="H30" s="20">
         <v>2020</v>
       </c>
-      <c r="H30" s="20">
-        <v>2019</v>
-      </c>
-      <c r="I30" s="77">
-        <v>11925000</v>
+      <c r="I30" s="60">
+        <v>0.93</v>
       </c>
       <c r="J30" s="70" t="s">
-        <v>141</v>
+        <v>286</v>
       </c>
       <c r="K30" s="60">
-        <v>2035</v>
+        <v>2031</v>
       </c>
       <c r="L30" s="74">
-        <v>0.75</v>
+        <v>0.10800000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="60" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C31" s="60" t="s">
-        <v>209</v>
-      </c>
-      <c r="D31" s="26">
-        <v>2050</v>
+        <v>213</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>66</v>
       </c>
       <c r="F31" s="60" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G31" s="60">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="H31" s="20">
-        <v>2020</v>
+        <v>2010</v>
       </c>
       <c r="I31" s="60">
-        <v>0.93</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="J31" s="70" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K31" s="60">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="L31" s="74">
-        <v>0.10800000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="60" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C32" s="60" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E32" s="26" t="s">
         <v>66</v>
       </c>
       <c r="F32" s="60" t="s">
-        <v>281</v>
-      </c>
-      <c r="G32" s="60">
-        <v>2020</v>
+        <v>283</v>
       </c>
       <c r="H32" s="20">
-        <v>2010</v>
+        <v>2000</v>
       </c>
       <c r="I32" s="60">
-        <v>0.76300000000000001</v>
+        <f>2650/2000</f>
+        <v>1.325</v>
       </c>
       <c r="J32" s="70" t="s">
         <v>287</v>
@@ -11502,43 +11500,49 @@
         <v>2030</v>
       </c>
       <c r="L32" s="74">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="60" customFormat="1">
       <c r="A33" s="60" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C33" s="60" t="s">
-        <v>216</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>66</v>
+        <v>222</v>
+      </c>
+      <c r="D33" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E33" s="60" t="s">
+        <v>282</v>
       </c>
       <c r="F33" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="H33" s="20">
-        <v>2000</v>
+      <c r="G33" s="60">
+        <v>2020</v>
+      </c>
+      <c r="H33" s="60">
+        <v>1990</v>
       </c>
       <c r="I33" s="60">
-        <f>2650/2000</f>
-        <v>1.325</v>
-      </c>
-      <c r="J33" s="70" t="s">
-        <v>287</v>
+        <f>7000000/(1-0.68)</f>
+        <v>21875000.000000004</v>
+      </c>
+      <c r="J33" s="60" t="s">
+        <v>141</v>
       </c>
       <c r="K33" s="60">
         <v>2030</v>
       </c>
       <c r="L33" s="74">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="60" customFormat="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="60" t="s">
         <v>220</v>
       </c>
@@ -11571,27 +11575,27 @@
         <v>141</v>
       </c>
       <c r="K34" s="60">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="L34" s="74">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="60" t="s">
-        <v>220</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>221</v>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="60" customFormat="1">
+      <c r="A35" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B35" s="60" t="s">
+        <v>303</v>
       </c>
       <c r="C35" s="60" t="s">
-        <v>222</v>
+        <v>304</v>
       </c>
       <c r="D35" s="26">
         <v>2050</v>
       </c>
-      <c r="E35" s="60" t="s">
-        <v>282</v>
+      <c r="E35" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="F35" s="60" t="s">
         <v>283</v>
@@ -11600,37 +11604,36 @@
         <v>2020</v>
       </c>
       <c r="H35" s="60">
-        <v>1990</v>
+        <v>2005</v>
       </c>
       <c r="I35" s="60">
-        <f>7000000/(1-0.68)</f>
-        <v>21875000.000000004</v>
-      </c>
-      <c r="J35" s="60" t="s">
-        <v>141</v>
+        <v>843</v>
+      </c>
+      <c r="J35" s="70" t="s">
+        <v>308</v>
       </c>
       <c r="K35" s="60">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="L35" s="74">
-        <v>0.9</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="60" customFormat="1">
       <c r="A36" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B36" s="60" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C36" s="60" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D36" s="26">
         <v>2050</v>
       </c>
-      <c r="E36" s="26" t="s">
-        <v>66</v>
+      <c r="E36" s="60" t="s">
+        <v>282</v>
       </c>
       <c r="F36" s="60" t="s">
         <v>283</v>
@@ -11642,166 +11645,163 @@
         <v>2005</v>
       </c>
       <c r="I36" s="60">
-        <v>843</v>
-      </c>
-      <c r="J36" s="70" t="s">
-        <v>309</v>
+        <f>6332981/(1-0.63)</f>
+        <v>17116164.864864863</v>
+      </c>
+      <c r="J36" s="60" t="s">
+        <v>141</v>
       </c>
       <c r="K36" s="60">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L36" s="74">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="60" customFormat="1">
-      <c r="A37" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B37" s="60" t="s">
-        <v>307</v>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="60" t="s">
+        <v>225</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="C37" s="60" t="s">
-        <v>308</v>
+        <v>227</v>
       </c>
       <c r="D37" s="26">
         <v>2050</v>
       </c>
-      <c r="E37" s="60" t="s">
+      <c r="E37" s="26" t="s">
         <v>282</v>
       </c>
       <c r="F37" s="60" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G37" s="60">
-        <v>2020</v>
-      </c>
-      <c r="H37" s="60">
-        <v>2005</v>
-      </c>
-      <c r="I37" s="60">
-        <f>6332981/(1-0.63)</f>
-        <v>17116164.864864863</v>
+        <v>2019</v>
+      </c>
+      <c r="H37" s="20">
+        <v>2010</v>
+      </c>
+      <c r="I37" s="75">
+        <v>3734024</v>
       </c>
       <c r="J37" s="60" t="s">
         <v>141</v>
       </c>
       <c r="K37" s="60">
-        <v>2030</v>
+        <v>2045</v>
       </c>
       <c r="L37" s="74">
         <v>0.9</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="60" t="s">
-        <v>225</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C38" s="60" t="s">
-        <v>227</v>
+    <row r="38" spans="1:12" s="60" customFormat="1">
+      <c r="A38" s="67" t="s">
+        <v>318</v>
+      </c>
+      <c r="B38" s="67" t="s">
+        <v>319</v>
+      </c>
+      <c r="C38" s="67" t="s">
+        <v>320</v>
       </c>
       <c r="D38" s="26">
         <v>2050</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="E38" s="60" t="s">
         <v>282</v>
       </c>
       <c r="F38" s="60" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G38" s="60">
-        <v>2019</v>
-      </c>
-      <c r="H38" s="20">
-        <v>2010</v>
-      </c>
-      <c r="I38" s="75">
-        <v>3734024</v>
+        <v>2021</v>
+      </c>
+      <c r="H38" s="60">
+        <v>2013</v>
+      </c>
+      <c r="I38" s="60">
+        <v>102</v>
       </c>
       <c r="J38" s="60" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="K38" s="60">
-        <v>2045</v>
+        <v>2030</v>
       </c>
       <c r="L38" s="74">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="60" customFormat="1">
-      <c r="A39" s="67" t="s">
-        <v>319</v>
-      </c>
-      <c r="B39" s="67" t="s">
-        <v>320</v>
-      </c>
-      <c r="C39" s="67" t="s">
-        <v>321</v>
-      </c>
-      <c r="D39" s="26">
-        <v>2050</v>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C39" s="60" t="s">
+        <v>219</v>
       </c>
       <c r="E39" s="60" t="s">
-        <v>282</v>
+        <v>66</v>
       </c>
       <c r="F39" s="60" t="s">
         <v>283</v>
       </c>
       <c r="G39" s="60">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="H39" s="60">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="I39" s="60">
-        <v>102</v>
+        <v>0.82</v>
       </c>
       <c r="J39" s="60" t="s">
-        <v>128</v>
+        <v>286</v>
       </c>
       <c r="K39" s="60">
         <v>2030</v>
       </c>
       <c r="L39" s="74">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="60" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="C40" s="60" t="s">
-        <v>219</v>
-      </c>
-      <c r="E40" s="60" t="s">
-        <v>66</v>
+        <v>230</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>282</v>
       </c>
       <c r="F40" s="60" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G40" s="60">
-        <v>2020</v>
-      </c>
-      <c r="H40" s="60">
-        <v>2015</v>
-      </c>
-      <c r="I40" s="60">
-        <v>0.82</v>
+        <v>2018</v>
+      </c>
+      <c r="H40" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I40" s="75">
+        <v>21445571</v>
       </c>
       <c r="J40" s="60" t="s">
-        <v>286</v>
+        <v>141</v>
       </c>
       <c r="K40" s="60">
         <v>2030</v>
       </c>
       <c r="L40" s="74">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -11833,80 +11833,83 @@
         <v>141</v>
       </c>
       <c r="K41" s="60">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="L41" s="74">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="60" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C42" s="60" t="s">
-        <v>230</v>
+        <v>233</v>
+      </c>
+      <c r="D42" s="26">
+        <v>2045</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>282</v>
       </c>
       <c r="F42" s="60" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G42" s="60">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="H42" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I42" s="75">
-        <v>21445571</v>
+        <v>2016</v>
+      </c>
+      <c r="I42" s="2">
+        <v>2.2165439930000002</v>
       </c>
       <c r="J42" s="60" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="K42" s="60">
-        <v>2050</v>
+        <v>2045</v>
       </c>
       <c r="L42" s="74">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="60" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C43" s="60" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D43" s="26">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="E43" s="26" t="s">
         <v>282</v>
       </c>
       <c r="F43" s="60" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G43" s="60">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="H43" s="20">
-        <v>2016</v>
-      </c>
-      <c r="I43" s="2">
-        <v>2.2165439930000002</v>
+        <v>2005</v>
+      </c>
+      <c r="I43" s="82">
+        <v>6976930.1319702603</v>
       </c>
       <c r="J43" s="60" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="K43" s="60">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="L43" s="74">
         <v>1</v>
@@ -11914,40 +11917,40 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="60" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C44" s="60" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D44" s="26">
-        <v>2040</v>
+        <v>2050</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>282</v>
+        <v>66</v>
       </c>
       <c r="F44" s="60" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G44" s="60">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="H44" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I44" s="82">
-        <v>6976930.1319702603</v>
+        <v>2017</v>
+      </c>
+      <c r="I44" s="60">
+        <v>2.06</v>
       </c>
       <c r="J44" s="60" t="s">
-        <v>141</v>
+        <v>286</v>
       </c>
       <c r="K44" s="60">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="L44" s="74">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -11982,48 +11985,49 @@
         <v>286</v>
       </c>
       <c r="K45" s="60">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="L45" s="74">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="60" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C46" s="60" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D46" s="26">
         <v>2050</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>66</v>
+        <v>282</v>
       </c>
       <c r="F46" s="60" t="s">
         <v>283</v>
       </c>
       <c r="G46" s="60">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H46" s="20">
-        <v>2017</v>
-      </c>
-      <c r="I46" s="60">
-        <v>2.06</v>
+        <v>2010</v>
+      </c>
+      <c r="I46" s="75">
+        <f>60736086+1597157</f>
+        <v>62333243</v>
       </c>
       <c r="J46" s="60" t="s">
-        <v>286</v>
+        <v>141</v>
       </c>
       <c r="K46" s="60">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="L46" s="74">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -12059,21 +12063,21 @@
         <v>141</v>
       </c>
       <c r="K47" s="60">
-        <v>2035</v>
+        <v>2040</v>
       </c>
       <c r="L47" s="74">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="60" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C48" s="60" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D48" s="26">
         <v>2050</v>
@@ -12085,40 +12089,39 @@
         <v>283</v>
       </c>
       <c r="G48" s="60">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="H48" s="20">
-        <v>2010</v>
-      </c>
-      <c r="I48" s="75">
-        <f>60736086+1597157</f>
-        <v>62333243</v>
+        <v>2005</v>
+      </c>
+      <c r="I48" s="85">
+        <v>16557441</v>
       </c>
       <c r="J48" s="60" t="s">
         <v>141</v>
       </c>
       <c r="K48" s="60">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="L48" s="74">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="60" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C49" s="60" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D49" s="26">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>282</v>
+        <v>66</v>
       </c>
       <c r="F49" s="60" t="s">
         <v>283</v>
@@ -12127,106 +12130,106 @@
         <v>2020</v>
       </c>
       <c r="H49" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I49" s="85">
-        <v>16557441</v>
+        <v>2010</v>
+      </c>
+      <c r="I49" s="60">
+        <v>0.47</v>
       </c>
       <c r="J49" s="60" t="s">
-        <v>141</v>
+        <v>287</v>
       </c>
       <c r="K49" s="60">
         <v>2030</v>
       </c>
       <c r="L49" s="74">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="60" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C50" s="60" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D50" s="26">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>66</v>
+        <v>282</v>
       </c>
       <c r="F50" s="60" t="s">
         <v>283</v>
       </c>
       <c r="G50" s="60">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H50" s="20">
-        <v>2010</v>
-      </c>
-      <c r="I50" s="60">
-        <v>0.47</v>
+        <v>2005</v>
+      </c>
+      <c r="I50" s="75">
+        <v>26566330</v>
       </c>
       <c r="J50" s="60" t="s">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="K50" s="60">
         <v>2030</v>
       </c>
       <c r="L50" s="74">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="60" customFormat="1">
       <c r="A51" s="60" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C51" s="60" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D51" s="26">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>282</v>
+        <v>66</v>
       </c>
       <c r="F51" s="60" t="s">
         <v>283</v>
       </c>
       <c r="G51" s="60">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="H51" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I51" s="75">
-        <v>26566330</v>
+        <v>2019</v>
+      </c>
+      <c r="I51" s="86">
+        <v>0.80243130614229874</v>
       </c>
       <c r="J51" s="60" t="s">
-        <v>141</v>
+        <v>287</v>
       </c>
       <c r="K51" s="60">
         <v>2030</v>
       </c>
       <c r="L51" s="74">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="60" customFormat="1">
       <c r="A52" s="60" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C52" s="60" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D52" s="26">
         <v>2050</v>
@@ -12241,10 +12244,10 @@
         <v>2020</v>
       </c>
       <c r="H52" s="20">
-        <v>2019</v>
+        <v>2007</v>
       </c>
       <c r="I52" s="86">
-        <v>0.80243130614229874</v>
+        <v>0.98420553538837829</v>
       </c>
       <c r="J52" s="60" t="s">
         <v>287</v>
@@ -12256,15 +12259,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="60" customFormat="1">
+    <row r="53" spans="1:12">
       <c r="A53" s="60" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C53" s="60" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D53" s="26">
         <v>2050</v>
@@ -12276,25 +12279,25 @@
         <v>283</v>
       </c>
       <c r="G53" s="60">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H53" s="20">
-        <v>2007</v>
-      </c>
-      <c r="I53" s="86">
-        <v>0.98420553538837829</v>
+        <v>2018</v>
+      </c>
+      <c r="I53" s="60">
+        <v>5.162928</v>
       </c>
       <c r="J53" s="60" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K53" s="60">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L53" s="74">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="60" customFormat="1">
       <c r="A54" s="60" t="s">
         <v>253</v>
       </c>
@@ -12326,21 +12329,21 @@
         <v>286</v>
       </c>
       <c r="K54" s="60">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L54" s="74">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" s="60" customFormat="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" s="60" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C55" s="60" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="D55" s="26">
         <v>2050</v>
@@ -12352,16 +12355,16 @@
         <v>283</v>
       </c>
       <c r="G55" s="60">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="H55" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I55" s="60">
-        <v>5.162928</v>
+        <v>2019</v>
+      </c>
+      <c r="I55" s="86">
+        <v>0.46760301224942979</v>
       </c>
       <c r="J55" s="60" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K55" s="60">
         <v>2030</v>
@@ -12372,16 +12375,13 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="60" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C56" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D56" s="26">
-        <v>2050</v>
+        <v>267</v>
       </c>
       <c r="E56" s="26" t="s">
         <v>66</v>
@@ -12390,16 +12390,16 @@
         <v>283</v>
       </c>
       <c r="G56" s="60">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H56" s="20">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="I56" s="86">
-        <v>0.46760301224942979</v>
+        <v>2.9</v>
       </c>
       <c r="J56" s="60" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K56" s="60">
         <v>2030</v>
@@ -12408,16 +12408,17 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" s="60" customFormat="1">
       <c r="A57" s="60" t="s">
-        <v>265</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>266</v>
+        <v>293</v>
+      </c>
+      <c r="B57" s="60" t="s">
+        <v>294</v>
       </c>
       <c r="C57" s="60" t="s">
-        <v>267</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="D57" s="26"/>
       <c r="E57" s="26" t="s">
         <v>66</v>
       </c>
@@ -12431,7 +12432,7 @@
         <v>2018</v>
       </c>
       <c r="I57" s="86">
-        <v>2.9</v>
+        <v>1.69</v>
       </c>
       <c r="J57" s="60" t="s">
         <v>286</v>
@@ -12440,20 +12441,19 @@
         <v>2030</v>
       </c>
       <c r="L57" s="74">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" s="60" customFormat="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="60" t="s">
-        <v>294</v>
-      </c>
-      <c r="B58" s="60" t="s">
-        <v>295</v>
+        <v>269</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>270</v>
       </c>
       <c r="C58" s="60" t="s">
-        <v>296</v>
-      </c>
-      <c r="D58" s="26"/>
+        <v>271</v>
+      </c>
       <c r="E58" s="26" t="s">
         <v>66</v>
       </c>
@@ -12467,7 +12467,7 @@
         <v>2018</v>
       </c>
       <c r="I58" s="86">
-        <v>1.69</v>
+        <v>0.42172199999999999</v>
       </c>
       <c r="J58" s="60" t="s">
         <v>286</v>
@@ -12476,18 +12476,18 @@
         <v>2030</v>
       </c>
       <c r="L58" s="74">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="60" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C59" s="60" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="E59" s="26" t="s">
         <v>66</v>
@@ -12496,13 +12496,13 @@
         <v>283</v>
       </c>
       <c r="G59" s="60">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="H59" s="20">
         <v>2018</v>
       </c>
       <c r="I59" s="86">
-        <v>0.42172199999999999</v>
+        <v>0.315911</v>
       </c>
       <c r="J59" s="60" t="s">
         <v>286</v>
@@ -12511,97 +12511,100 @@
         <v>2030</v>
       </c>
       <c r="L59" s="74">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
-      <c r="A60" s="60" t="s">
-        <v>272</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="C60" s="60" t="s">
-        <v>274</v>
-      </c>
-      <c r="E60" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F60" s="60" t="s">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="60" customFormat="1">
+      <c r="A60" s="88" t="s">
+        <v>309</v>
+      </c>
+      <c r="B60" s="88" t="s">
+        <v>310</v>
+      </c>
+      <c r="C60" s="88" t="s">
+        <v>311</v>
+      </c>
+      <c r="D60" s="88">
+        <v>2050</v>
+      </c>
+      <c r="E60" s="88" t="s">
+        <v>282</v>
+      </c>
+      <c r="F60" s="88" t="s">
+        <v>281</v>
+      </c>
+      <c r="G60" s="88">
+        <v>2020</v>
+      </c>
+      <c r="H60" s="88">
+        <v>2005</v>
+      </c>
+      <c r="I60" s="88">
+        <v>11.641638960259289</v>
+      </c>
+      <c r="J60" s="88" t="s">
+        <v>128</v>
+      </c>
+      <c r="K60" s="88">
+        <v>2050</v>
+      </c>
+      <c r="L60" s="89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="60" customFormat="1">
+      <c r="A61" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B61" s="60" t="s">
+        <v>313</v>
+      </c>
+      <c r="C61" s="60" t="s">
+        <v>314</v>
+      </c>
+      <c r="D61" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="F61" s="60" t="s">
         <v>283</v>
       </c>
-      <c r="G60" s="60">
+      <c r="G61" s="60">
         <v>2020</v>
       </c>
-      <c r="H60" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I60" s="86">
-        <v>0.315911</v>
-      </c>
-      <c r="J60" s="60" t="s">
-        <v>286</v>
-      </c>
-      <c r="K60" s="60">
+      <c r="H61" s="20">
+        <v>2010</v>
+      </c>
+      <c r="I61" s="60">
+        <v>69124235.200000003</v>
+      </c>
+      <c r="J61" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="K61" s="60">
         <v>2030</v>
       </c>
-      <c r="L60" s="74">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="60" customFormat="1">
-      <c r="A61" s="88" t="s">
-        <v>310</v>
-      </c>
-      <c r="B61" s="88" t="s">
-        <v>311</v>
-      </c>
-      <c r="C61" s="88" t="s">
-        <v>312</v>
-      </c>
-      <c r="D61" s="88">
-        <v>2050</v>
-      </c>
-      <c r="E61" s="88" t="s">
-        <v>282</v>
-      </c>
-      <c r="F61" s="88" t="s">
-        <v>281</v>
-      </c>
-      <c r="G61" s="88">
-        <v>2020</v>
-      </c>
-      <c r="H61" s="88">
-        <v>2005</v>
-      </c>
-      <c r="I61" s="88">
-        <v>11.641638960259289</v>
-      </c>
-      <c r="J61" s="88" t="s">
-        <v>128</v>
-      </c>
-      <c r="K61" s="88">
-        <v>2050</v>
-      </c>
-      <c r="L61" s="89">
-        <v>1</v>
+      <c r="L61" s="74">
+        <v>0.6</v>
       </c>
     </row>
     <row r="62" spans="1:12" s="60" customFormat="1">
-      <c r="A62" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="B62" s="60" t="s">
-        <v>314</v>
+      <c r="A62" s="60" t="s">
+        <v>275</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>276</v>
       </c>
       <c r="C62" s="60" t="s">
-        <v>315</v>
+        <v>277</v>
       </c>
       <c r="D62" s="26">
         <v>2050</v>
       </c>
       <c r="E62" s="26" t="s">
-        <v>282</v>
+        <v>66</v>
       </c>
       <c r="F62" s="60" t="s">
         <v>283</v>
@@ -12610,16 +12613,16 @@
         <v>2020</v>
       </c>
       <c r="H62" s="20">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="I62" s="60">
-        <v>69124235.200000003</v>
+        <v>0.78</v>
       </c>
       <c r="J62" s="60" t="s">
-        <v>141</v>
+        <v>287</v>
       </c>
       <c r="K62" s="60">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="L62" s="74">
         <v>0.6</v>
@@ -12657,21 +12660,21 @@
         <v>287</v>
       </c>
       <c r="K63" s="60">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="L63" s="74">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="64" spans="1:12" s="60" customFormat="1">
-      <c r="A64" s="60" t="s">
-        <v>275</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>276</v>
+      <c r="A64" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B64" s="60" t="s">
+        <v>316</v>
       </c>
       <c r="C64" s="60" t="s">
-        <v>277</v>
+        <v>317</v>
       </c>
       <c r="D64" s="26">
         <v>2050</v>
@@ -12686,30 +12689,30 @@
         <v>2020</v>
       </c>
       <c r="H64" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I64" s="60">
-        <v>0.78</v>
+        <v>2018</v>
+      </c>
+      <c r="I64" s="86">
+        <v>0.315911</v>
       </c>
       <c r="J64" s="60" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K64" s="60">
         <v>2030</v>
       </c>
       <c r="L64" s="74">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" s="60" customFormat="1">
-      <c r="A65" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="B65" s="60" t="s">
-        <v>317</v>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="60" t="s">
+        <v>278</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="C65" s="60" t="s">
-        <v>318</v>
+        <v>280</v>
       </c>
       <c r="D65" s="26">
         <v>2050</v>
@@ -12724,56 +12727,18 @@
         <v>2020</v>
       </c>
       <c r="H65" s="20">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="I65" s="86">
-        <v>0.315911</v>
+        <v>0.88086205923584682</v>
       </c>
       <c r="J65" s="60" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K65" s="60">
         <v>2030</v>
       </c>
       <c r="L65" s="74">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12">
-      <c r="A66" s="60" t="s">
-        <v>278</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="C66" s="60" t="s">
-        <v>280</v>
-      </c>
-      <c r="D66" s="26">
-        <v>2050</v>
-      </c>
-      <c r="E66" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F66" s="60" t="s">
-        <v>283</v>
-      </c>
-      <c r="G66" s="60">
-        <v>2020</v>
-      </c>
-      <c r="H66" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I66" s="86">
-        <v>0.88086205923584682</v>
-      </c>
-      <c r="J66" s="60" t="s">
-        <v>287</v>
-      </c>
-      <c r="K66" s="60">
-        <v>2030</v>
-      </c>
-      <c r="L66" s="74">
         <v>0.8</v>
       </c>
     </row>
@@ -12793,17 +12758,17 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.7109375" style="51" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" customWidth="1"/>
-    <col min="8" max="8" width="87.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="38" t="s">
         <v>12</v>
       </c>
@@ -12863,7 +12828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2">
+    <row r="4" spans="1:6" ht="45">
       <c r="A4" s="40" t="s">
         <v>13</v>
       </c>
@@ -12883,7 +12848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8">
+    <row r="5" spans="1:6" ht="30">
       <c r="A5" s="40" t="s">
         <v>13</v>
       </c>
@@ -12903,7 +12868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.2">
+    <row r="6" spans="1:6" ht="60">
       <c r="A6" s="40" t="s">
         <v>13</v>
       </c>
@@ -12963,7 +12928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8">
+    <row r="9" spans="1:6" ht="45">
       <c r="A9" s="40" t="s">
         <v>13</v>
       </c>
@@ -13063,7 +13028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.8">
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="40" t="s">
         <v>13</v>
       </c>
@@ -13143,7 +13108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.8">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="31" t="s">
         <v>15</v>
       </c>
@@ -13163,7 +13128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="31" t="s">
         <v>15</v>
       </c>
@@ -13183,7 +13148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="31" t="s">
         <v>15</v>
       </c>
@@ -13203,7 +13168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8">
+    <row r="21" spans="1:6" ht="30">
       <c r="A21" s="31" t="s">
         <v>15</v>
       </c>
@@ -13223,7 +13188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="31" t="s">
         <v>15</v>
       </c>
@@ -13243,7 +13208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8">
+    <row r="23" spans="1:6" ht="30">
       <c r="A23" s="31" t="s">
         <v>15</v>
       </c>
@@ -13263,7 +13228,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="43.2">
+    <row r="24" spans="1:6" ht="45">
       <c r="A24" s="31" t="s">
         <v>15</v>
       </c>
@@ -13283,7 +13248,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28.8">
+    <row r="25" spans="1:6" ht="30">
       <c r="A25" s="31" t="s">
         <v>15</v>
       </c>
@@ -13303,7 +13268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.8">
+    <row r="26" spans="1:6" ht="30">
       <c r="A26" s="31" t="s">
         <v>15</v>
       </c>
@@ -13323,7 +13288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28.8">
+    <row r="27" spans="1:6" ht="30">
       <c r="A27" s="31" t="s">
         <v>15</v>
       </c>
@@ -13343,7 +13308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.8">
+    <row r="28" spans="1:6" ht="30">
       <c r="A28" s="31" t="s">
         <v>15</v>
       </c>
@@ -13363,7 +13328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.8">
+    <row r="29" spans="1:6" ht="30">
       <c r="A29" s="31" t="s">
         <v>15</v>
       </c>
@@ -13383,7 +13348,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.8">
+    <row r="30" spans="1:6" ht="30">
       <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
@@ -13403,7 +13368,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43.2">
+    <row r="31" spans="1:6" ht="45">
       <c r="A31" s="31" t="s">
         <v>15</v>
       </c>
@@ -13423,7 +13388,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="28.8">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="31" t="s">
         <v>15</v>
       </c>
@@ -13443,7 +13408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="31" t="s">
         <v>15</v>
       </c>
@@ -13463,7 +13428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="31" t="s">
         <v>15</v>
       </c>
@@ -13483,7 +13448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8">
+    <row r="35" spans="1:6" ht="30">
       <c r="A35" s="31" t="s">
         <v>15</v>
       </c>
@@ -13503,7 +13468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8">
+    <row r="36" spans="1:6" ht="30">
       <c r="A36" s="31" t="s">
         <v>15</v>
       </c>
@@ -13523,7 +13488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8">
+    <row r="37" spans="1:6" ht="30">
       <c r="A37" s="31" t="s">
         <v>15</v>
       </c>
@@ -13543,7 +13508,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="43.2">
+    <row r="38" spans="1:6" ht="45">
       <c r="A38" s="31" t="s">
         <v>15</v>
       </c>
@@ -13563,7 +13528,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8">
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="31" t="s">
         <v>15</v>
       </c>
@@ -13583,7 +13548,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28.8">
+    <row r="40" spans="1:6" ht="30">
       <c r="A40" s="31" t="s">
         <v>15</v>
       </c>
@@ -13603,7 +13568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="28.8">
+    <row r="41" spans="1:6" ht="30">
       <c r="A41" s="31" t="s">
         <v>15</v>
       </c>
@@ -13623,7 +13588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="28.8">
+    <row r="42" spans="1:6" ht="30">
       <c r="A42" s="31" t="s">
         <v>15</v>
       </c>
@@ -13643,7 +13608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.8">
+    <row r="43" spans="1:6" ht="30">
       <c r="A43" s="31" t="s">
         <v>15</v>
       </c>
@@ -13663,7 +13628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="28.8">
+    <row r="44" spans="1:6" ht="30">
       <c r="A44" s="31" t="s">
         <v>15</v>
       </c>
@@ -13683,7 +13648,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="43.2">
+    <row r="45" spans="1:6" ht="45">
       <c r="A45" s="31" t="s">
         <v>15</v>
       </c>
@@ -13703,7 +13668,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="28.8">
+    <row r="46" spans="1:6" ht="30">
       <c r="A46" s="50" t="s">
         <v>74</v>
       </c>
@@ -13723,7 +13688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="28.8">
+    <row r="47" spans="1:6" ht="30">
       <c r="A47" s="50" t="s">
         <v>74</v>
       </c>
@@ -13743,7 +13708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="28.8">
+    <row r="48" spans="1:6" ht="30">
       <c r="A48" s="50" t="s">
         <v>74</v>
       </c>
@@ -13763,7 +13728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="28.8">
+    <row r="49" spans="1:6" ht="30">
       <c r="A49" s="50" t="s">
         <v>74</v>
       </c>
@@ -13783,7 +13748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="28.8">
+    <row r="50" spans="1:6" ht="30">
       <c r="A50" s="50" t="s">
         <v>74</v>
       </c>
@@ -13803,7 +13768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="28.8">
+    <row r="51" spans="1:6" ht="30">
       <c r="A51" s="44" t="s">
         <v>14</v>
       </c>
@@ -13823,7 +13788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="43.2">
+    <row r="52" spans="1:6" ht="60">
       <c r="A52" s="44" t="s">
         <v>14</v>
       </c>
@@ -13883,7 +13848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="72">
+    <row r="55" spans="1:6" ht="75">
       <c r="A55" s="44" t="s">
         <v>14</v>
       </c>
@@ -13903,7 +13868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="72">
+    <row r="56" spans="1:6" ht="75">
       <c r="A56" s="44" t="s">
         <v>14</v>
       </c>
@@ -13943,7 +13908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="28.8">
+    <row r="58" spans="1:6" ht="30">
       <c r="A58" s="44" t="s">
         <v>14</v>
       </c>
@@ -13963,7 +13928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="43.2">
+    <row r="59" spans="1:6" ht="45">
       <c r="A59" s="45" t="s">
         <v>102</v>
       </c>
@@ -14001,12 +13966,12 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" style="60" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -14020,10 +13985,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="84" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="84" t="s">
         <v>290</v>
-      </c>
-      <c r="E1" s="84" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -14041,7 +14006,7 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E33" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>153911</v>
+        <v>45506</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -14059,7 +14024,7 @@
       </c>
       <c r="E3" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>198025</v>
+        <v>199516</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -14077,7 +14042,7 @@
       </c>
       <c r="E4" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>91511</v>
+        <v>136769</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -14095,7 +14060,7 @@
       </c>
       <c r="E5" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>120618</v>
+        <v>133933</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -14113,7 +14078,7 @@
       </c>
       <c r="E6" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>156977</v>
+        <v>165920</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -14131,7 +14096,7 @@
       </c>
       <c r="E7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>115292</v>
+        <v>114363</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -14149,7 +14114,7 @@
       </c>
       <c r="E8" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>190233</v>
+        <v>50344</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -14167,25 +14132,25 @@
       </c>
       <c r="E9" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>65699</v>
+        <v>181187</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="60" t="s">
+        <v>296</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="60" t="s">
         <v>298</v>
       </c>
-      <c r="C10" s="60" t="s">
-        <v>299</v>
-      </c>
       <c r="D10" s="60" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E10" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>119489</v>
+        <v>187913</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -14203,7 +14168,7 @@
       </c>
       <c r="E11" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>76429</v>
+        <v>181825</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -14221,7 +14186,7 @@
       </c>
       <c r="E12" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>36506</v>
+        <v>218982</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -14239,7 +14204,7 @@
       </c>
       <c r="E13" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>105945</v>
+        <v>174132</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -14257,7 +14222,7 @@
       </c>
       <c r="E14" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>226903</v>
+        <v>62636</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -14275,7 +14240,7 @@
       </c>
       <c r="E15" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>114503</v>
+        <v>44212</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -14293,7 +14258,7 @@
       </c>
       <c r="E16" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>53796</v>
+        <v>151935</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -14311,25 +14276,25 @@
       </c>
       <c r="E17" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>188664</v>
+        <v>180016</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="60" t="s">
+        <v>299</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="60" t="s">
         <v>301</v>
       </c>
-      <c r="C18" s="60" t="s">
-        <v>302</v>
-      </c>
       <c r="D18" s="60" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E18" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>102983</v>
+        <v>124406</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -14347,7 +14312,7 @@
       </c>
       <c r="E19" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>104205</v>
+        <v>205404</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -14365,7 +14330,7 @@
       </c>
       <c r="E20" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>179611</v>
+        <v>238027</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -14383,7 +14348,7 @@
       </c>
       <c r="E21" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>105482</v>
+        <v>59096</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -14401,7 +14366,7 @@
       </c>
       <c r="E22" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>177985</v>
+        <v>124090</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -14419,7 +14384,7 @@
       </c>
       <c r="E23" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>189072</v>
+        <v>113395</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -14437,7 +14402,7 @@
       </c>
       <c r="E24" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>170018</v>
+        <v>155166</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -14455,7 +14420,7 @@
       </c>
       <c r="E25" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>129927</v>
+        <v>120864</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -14473,7 +14438,7 @@
       </c>
       <c r="E26" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>215672</v>
+        <v>130471</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -14491,7 +14456,7 @@
       </c>
       <c r="E27" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>103247</v>
+        <v>133737</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -14509,7 +14474,7 @@
       </c>
       <c r="E28" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>52867</v>
+        <v>91663</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -14527,61 +14492,61 @@
       </c>
       <c r="E29" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>165114</v>
+        <v>56626</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="60" t="s">
+        <v>302</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="60" t="s">
         <v>304</v>
       </c>
-      <c r="C30" s="60" t="s">
-        <v>305</v>
-      </c>
       <c r="D30" s="60" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E30" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>235427</v>
+        <v>61487</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="60" t="s">
+        <v>318</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="60" t="s">
         <v>320</v>
       </c>
-      <c r="C31" s="60" t="s">
-        <v>321</v>
-      </c>
       <c r="D31" s="60" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E31" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>233647</v>
+        <v>93156</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="60" t="s">
+        <v>305</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="60" t="s">
         <v>307</v>
       </c>
-      <c r="C32" s="60" t="s">
-        <v>308</v>
-      </c>
       <c r="D32" s="60" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E32" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>108840</v>
+        <v>189399</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -14599,7 +14564,7 @@
       </c>
       <c r="E33" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>175723</v>
+        <v>135844</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -14617,7 +14582,7 @@
       </c>
       <c r="E34" s="60">
         <f t="shared" ref="E34:E54" ca="1" si="1">RANDBETWEEN(35000,250000)</f>
-        <v>198058</v>
+        <v>56971</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -14635,7 +14600,7 @@
       </c>
       <c r="E35" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>238784</v>
+        <v>115918</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -14653,7 +14618,7 @@
       </c>
       <c r="E36" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>85880</v>
+        <v>46010</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -14671,7 +14636,7 @@
       </c>
       <c r="E37" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>223488</v>
+        <v>193522</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -14689,7 +14654,7 @@
       </c>
       <c r="E38" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>150288</v>
+        <v>86270</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -14707,7 +14672,7 @@
       </c>
       <c r="E39" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>103903</v>
+        <v>63017</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -14725,7 +14690,7 @@
       </c>
       <c r="E40" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>51284</v>
+        <v>95709</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -14743,7 +14708,7 @@
       </c>
       <c r="E41" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>90483</v>
+        <v>120368</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -14761,7 +14726,7 @@
       </c>
       <c r="E42" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>239548</v>
+        <v>60032</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -14779,7 +14744,7 @@
       </c>
       <c r="E43" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>215326</v>
+        <v>82483</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="60" customFormat="1">
@@ -14797,7 +14762,7 @@
       </c>
       <c r="E44" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>224097</v>
+        <v>136772</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -14815,7 +14780,7 @@
       </c>
       <c r="E45" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>52940</v>
+        <v>112273</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -14833,25 +14798,25 @@
       </c>
       <c r="E46" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>149814</v>
+        <v>45832</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
+        <v>293</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="C47" t="s">
         <v>295</v>
       </c>
-      <c r="C47" t="s">
-        <v>296</v>
-      </c>
       <c r="D47" s="60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E47" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>57195</v>
+        <v>63384</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -14869,7 +14834,7 @@
       </c>
       <c r="E48" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>227052</v>
+        <v>170828</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -14887,43 +14852,43 @@
       </c>
       <c r="E49" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>232742</v>
+        <v>41284</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
+        <v>309</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" t="s">
         <v>311</v>
       </c>
-      <c r="C50" t="s">
-        <v>312</v>
-      </c>
       <c r="D50" s="60" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E50" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>43918</v>
+        <v>55233</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
+        <v>312</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" t="s">
         <v>314</v>
       </c>
-      <c r="C51" t="s">
-        <v>315</v>
-      </c>
       <c r="D51" s="60" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E51" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>95541</v>
+        <v>71174</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -14941,25 +14906,25 @@
       </c>
       <c r="E52" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>192147</v>
+        <v>181804</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
+        <v>315</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" t="s">
         <v>317</v>
       </c>
-      <c r="C53" t="s">
-        <v>318</v>
-      </c>
       <c r="D53" s="60" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E53" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>145112</v>
+        <v>50955</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -14977,7 +14942,7 @@
       </c>
       <c r="E54" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>43111</v>
+        <v>157865</v>
       </c>
     </row>
   </sheetData>
@@ -14997,7 +14962,7 @@
       <selection sqref="A1:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>